<commit_message>
Attendance Module is optimized
</commit_message>
<xml_diff>
--- a/src/test/resources/Datas/Testdatas.xlsx
+++ b/src/test/resources/Datas/Testdatas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7530" tabRatio="948" activeTab="2"/>
+    <workbookView windowWidth="19635" windowHeight="7530" tabRatio="948" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="76">
   <si>
     <t>TCID</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>TC_010</t>
-  </si>
-  <si>
-    <t>arjundel</t>
   </si>
   <si>
     <t>Attendancetype</t>
@@ -1366,8 +1363,8 @@
   <sheetPr/>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelCol="1"/>
@@ -1406,7 +1403,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" ht="20.25" spans="1:2">
@@ -1511,8 +1508,8 @@
   <sheetPr/>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1712,10 +1709,10 @@
         <v>32</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>21</v>
@@ -1738,8 +1735,8 @@
   <sheetPr/>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1753,7 +1750,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1764,7 +1761,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
@@ -1775,7 +1772,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -1786,7 +1783,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>5</v>
@@ -1797,7 +1794,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>5</v>
@@ -1808,7 +1805,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
@@ -1819,7 +1816,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1830,7 +1827,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>5</v>
@@ -1841,7 +1838,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>3</v>
@@ -1852,7 +1849,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>5</v>
@@ -1863,7 +1860,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>5</v>
@@ -1881,7 +1878,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -1895,10 +1892,10 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1909,7 +1906,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -1944,7 +1941,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1955,7 +1952,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
@@ -1966,7 +1963,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -1977,7 +1974,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>5</v>
@@ -2012,7 +2009,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2023,7 +2020,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
@@ -2034,7 +2031,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -2045,7 +2042,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>5</v>
@@ -2056,7 +2053,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>5</v>
@@ -2067,7 +2064,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
@@ -2078,7 +2075,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -2089,7 +2086,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>5</v>
@@ -2100,7 +2097,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>5</v>
@@ -2111,7 +2108,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>5</v>
@@ -2149,37 +2146,37 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>1</v>
@@ -2190,34 +2187,34 @@
         <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="D2" s="2">
         <v>33456</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L2" s="2" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Retry Analyzer is Implemented Properties config should be develop
</commit_message>
<xml_diff>
--- a/src/test/resources/Datas/Testdatas.xlsx
+++ b/src/test/resources/Datas/Testdatas.xlsx
@@ -4,24 +4,23 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7530" tabRatio="948" activeTab="3"/>
+    <workbookView windowWidth="19635" windowHeight="7530" tabRatio="948"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="4" r:id="rId1"/>
-    <sheet name="TC001_VerifyAppVersion" sheetId="5" r:id="rId2"/>
-    <sheet name="TC002_VerifyLogin" sheetId="2" r:id="rId3"/>
-    <sheet name="TC001_VerifyImagerequired" sheetId="7" r:id="rId4"/>
-    <sheet name="TC002_VerifyAttendance" sheetId="6" r:id="rId5"/>
-    <sheet name="TC001_VerifyDownloadcalls" sheetId="8" r:id="rId6"/>
-    <sheet name="TC001_VerifyResourcecentrefiles" sheetId="9" r:id="rId7"/>
-    <sheet name="TC001_VerifyVistorlogin" sheetId="10" r:id="rId8"/>
+    <sheet name="TC001_VerifyLogin" sheetId="2" r:id="rId2"/>
+    <sheet name="TC001_VerifyImagerequired" sheetId="7" r:id="rId3"/>
+    <sheet name="TC002_VerifyAttendance" sheetId="6" r:id="rId4"/>
+    <sheet name="TC001_VerifyDownloadcalls" sheetId="8" r:id="rId5"/>
+    <sheet name="TC001_VerifyResourcecentrefiles" sheetId="9" r:id="rId6"/>
+    <sheet name="TC001_VerifyVistorlogin" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="73">
   <si>
     <t>TCID</t>
   </si>
@@ -29,21 +28,18 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>TC001_VerifyAppVersion</t>
+    <t>TC001_VerifyLogin</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>TC001_VerifyImagerequired</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>TC002_VerifyLogin</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>TC001_VerifyImagerequired</t>
-  </si>
-  <si>
     <t>TC002_VerifyAttendance</t>
   </si>
   <si>
@@ -59,25 +55,19 @@
     <t>TC ID</t>
   </si>
   <si>
-    <t>Version</t>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Mobilenumber</t>
   </si>
   <si>
     <t>TC_001</t>
-  </si>
-  <si>
-    <t>V 3.1.4</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>Mobilenumber</t>
   </si>
   <si>
     <t>vishaldel</t>
@@ -261,7 +251,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,19 +305,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -491,7 +468,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,12 +490,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,137 +821,137 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1020,28 +991,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1361,98 +1323,74 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="44" style="15" customWidth="1"/>
-    <col min="2" max="2" width="34" style="15" customWidth="1"/>
-    <col min="3" max="16384" width="9.14285714285714" style="15"/>
+    <col min="1" max="1" width="44" style="13" customWidth="1"/>
+    <col min="2" max="2" width="16.1238095238095" style="13" customWidth="1"/>
+    <col min="3" max="16384" width="9.14285714285714" style="13"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" spans="1:2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="20.25" spans="1:2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="20.25" spans="1:2">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="20.25" spans="1:2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" ht="20.25" spans="1:2">
+      <c r="A5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" ht="20.25" spans="1:2">
-      <c r="A5" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="18" t="s">
+    <row r="6" ht="20.25" spans="1:2">
+      <c r="A6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="20.25" spans="1:2">
-      <c r="A6" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="7" ht="20.25" spans="1:2">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" ht="20.25" spans="1:2">
-      <c r="A8" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" ht="20.25" spans="1:2">
-      <c r="A9" s="20"/>
-      <c r="B9" s="18"/>
-    </row>
-    <row r="10" ht="20.25" spans="1:2">
-      <c r="A10" s="20"/>
-      <c r="B10" s="18"/>
-    </row>
-    <row r="11" ht="20.25" spans="1:2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="18"/>
-    </row>
-    <row r="12" ht="20.25" spans="1:2">
-      <c r="A12" s="20"/>
-      <c r="B12" s="18"/>
+      <c r="B7" s="16" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1463,53 +1401,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
-  <cols>
-    <col min="2" max="2" width="11.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="10.4285714285714" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1522,19 +1417,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -1542,186 +1437,186 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="F2" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="F3" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="F4" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" ht="16.5" spans="1:6">
       <c r="A6" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="F6" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" ht="16.5" spans="1:6">
       <c r="A9" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" ht="16.5" spans="1:6">
       <c r="A10" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="12"/>
       <c r="F10" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="F11" s="11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1730,13 +1625,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1747,10 +1642,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1758,112 +1653,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1872,13 +1767,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -1889,13 +1784,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1903,16 +1798,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1921,7 +1816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:C5"/>
@@ -1938,10 +1833,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1949,35 +1844,35 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -1989,7 +1884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:C10"/>
@@ -2006,10 +1901,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2017,101 +1912,101 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2120,13 +2015,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2143,40 +2038,40 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>1</v>
@@ -2184,43 +2079,43 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D2" s="2">
         <v>33456</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.Hardcoded Values is moved to Properties 2.Screenshot is captured in seperate folder. 3.Screenshot and Automation report is added in Mail.
</commit_message>
<xml_diff>
--- a/src/test/resources/Datas/Testdatas.xlsx
+++ b/src/test/resources/Datas/Testdatas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7530" tabRatio="948"/>
+    <workbookView windowWidth="19635" windowHeight="7530" tabRatio="948" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="75">
   <si>
     <t>TCID</t>
   </si>
@@ -112,7 +112,10 @@
     <t>TC_010</t>
   </si>
   <si>
-    <t>gyanedel</t>
+    <t>harikdel</t>
+  </si>
+  <si>
+    <t>824860691</t>
   </si>
   <si>
     <t>Attendancetype</t>
@@ -1328,8 +1331,8 @@
   <sheetPr/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelRow="6" outlineLevelCol="1"/>
@@ -1406,8 +1409,8 @@
   <sheetPr/>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1616,7 +1619,7 @@
         <v>18</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>3</v>
@@ -1634,7 +1637,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1648,7 +1651,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1659,7 +1662,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
@@ -1670,7 +1673,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>3</v>
@@ -1681,7 +1684,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>3</v>
@@ -1692,7 +1695,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>3</v>
@@ -1703,7 +1706,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>3</v>
@@ -1714,7 +1717,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>3</v>
@@ -1725,7 +1728,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>3</v>
@@ -1736,7 +1739,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>5</v>
@@ -1747,7 +1750,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>3</v>
@@ -1758,7 +1761,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>3</v>
@@ -1790,10 +1793,10 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1804,7 +1807,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -1839,7 +1842,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1850,7 +1853,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
@@ -1861,7 +1864,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>3</v>
@@ -1872,7 +1875,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>3</v>
@@ -1907,7 +1910,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1918,7 +1921,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
@@ -1929,7 +1932,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>3</v>
@@ -1940,7 +1943,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>3</v>
@@ -1951,7 +1954,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>3</v>
@@ -1962,7 +1965,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>3</v>
@@ -1973,7 +1976,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>3</v>
@@ -1984,7 +1987,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>3</v>
@@ -1995,7 +1998,7 @@
         <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>3</v>
@@ -2006,7 +2009,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>3</v>
@@ -2044,37 +2047,37 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>1</v>
@@ -2085,34 +2088,34 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D2" s="2">
         <v>33456</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L2" s="2" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
1.Hardcoded Values is moved to Properties 2.Screenshot is captured in seperate folder. 3.Screenshot and Automation report is added in Mail. 4. Baseclass is Desired Capabilities is Optimized.
</commit_message>
<xml_diff>
--- a/src/test/resources/Datas/Testdatas.xlsx
+++ b/src/test/resources/Datas/Testdatas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
   <si>
     <t>TCID</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>harikdel</t>
-  </si>
-  <si>
-    <t>824860691</t>
   </si>
   <si>
     <t>Attendancetype</t>
@@ -1410,7 +1407,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1619,7 +1616,7 @@
         <v>18</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>3</v>
@@ -1651,7 +1648,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1662,7 +1659,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
@@ -1673,7 +1670,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>3</v>
@@ -1684,7 +1681,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>3</v>
@@ -1695,7 +1692,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>3</v>
@@ -1706,7 +1703,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>3</v>
@@ -1717,7 +1714,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>3</v>
@@ -1728,7 +1725,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>3</v>
@@ -1739,7 +1736,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>5</v>
@@ -1750,7 +1747,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>3</v>
@@ -1761,7 +1758,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>3</v>
@@ -1793,10 +1790,10 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1807,7 +1804,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="b">
         <v>1</v>
@@ -1842,7 +1839,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1853,7 +1850,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
@@ -1864,7 +1861,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>3</v>
@@ -1875,7 +1872,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>3</v>
@@ -1910,7 +1907,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1921,7 +1918,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
@@ -1932,7 +1929,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>3</v>
@@ -1943,7 +1940,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>3</v>
@@ -1954,7 +1951,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>3</v>
@@ -1965,7 +1962,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>3</v>
@@ -1976,7 +1973,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>3</v>
@@ -1987,7 +1984,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>3</v>
@@ -1998,7 +1995,7 @@
         <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>3</v>
@@ -2009,7 +2006,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>3</v>
@@ -2047,37 +2044,37 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>1</v>
@@ -2088,34 +2085,34 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="D2" s="2">
         <v>33456</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L2" s="2" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
1.Call plan should be developed
</commit_message>
<xml_diff>
--- a/src/test/resources/Datas/Testdatas.xlsx
+++ b/src/test/resources/Datas/Testdatas.xlsx
@@ -14,13 +14,14 @@
     <sheet name="TC001_VerifyDownloadcalls" sheetId="8" r:id="rId5"/>
     <sheet name="TC001_VerifyResourcecentrefiles" sheetId="9" r:id="rId6"/>
     <sheet name="TC001_VerifyVistorlogin" sheetId="10" r:id="rId7"/>
+    <sheet name="TC001_VerifyUploadcall" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="77">
   <si>
     <t>TCID</t>
   </si>
@@ -52,6 +53,12 @@
     <t>TC001_VerifyVistorlogin</t>
   </si>
   <si>
+    <t>TC001_VerifyUploadcall</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
     <t>TC ID</t>
   </si>
   <si>
@@ -112,9 +119,6 @@
     <t>TC_010</t>
   </si>
   <si>
-    <t>harikdel</t>
-  </si>
-  <si>
     <t>Attendancetype</t>
   </si>
   <si>
@@ -242,6 +246,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>TargetID</t>
+  </si>
+  <si>
+    <t>38356</t>
   </si>
 </sst>
 </file>
@@ -954,26 +964,29 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1326,73 +1339,86 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelRow="6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="44" style="13" customWidth="1"/>
-    <col min="2" max="2" width="16.1238095238095" style="13" customWidth="1"/>
-    <col min="3" max="16384" width="9.14285714285714" style="13"/>
+    <col min="1" max="1" width="44" style="14" customWidth="1"/>
+    <col min="2" max="2" width="16.1238095238095" style="14" customWidth="1"/>
+    <col min="3" max="16384" width="9.14285714285714" style="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" spans="1:2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="20.25" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="20.25" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="20.25" spans="1:2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" ht="20.25" spans="1:2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" ht="20.25" spans="1:2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" ht="20.25" spans="1:2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="17" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" ht="20.25" spans="1:2">
+      <c r="A8" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" s="14" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1407,7 +1433,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B11" sqref="B11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1420,205 +1446,205 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="D2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="C4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="C5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="10" t="s">
+    <row r="6" ht="16.5" spans="1:6">
+      <c r="A6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="11" t="s">
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="11" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="16.5" spans="1:6">
-      <c r="A6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="10" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="C8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
+    <row r="9" ht="16.5" spans="1:6">
+      <c r="A9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="11" t="s">
+      <c r="C9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="11" t="s">
+    <row r="10" ht="16.5" spans="1:6">
+      <c r="A10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" ht="16.5" spans="1:6">
-      <c r="A9" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="10" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" ht="16.5" spans="1:6">
-      <c r="A10" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="C11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="11" t="s">
+      <c r="D11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1645,122 +1671,122 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1787,29 +1813,29 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="5" t="b">
+      <c r="A2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1836,50 +1862,50 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1893,7 +1919,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A1" sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1904,111 +1930,111 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2041,83 +2067,125 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:13">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="5">
+        <v>33456</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="2" max="2" width="16.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="2">
-        <v>33456</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1.Call plan is In Progress in JJ_test
</commit_message>
<xml_diff>
--- a/src/test/resources/Datas/Testdatas.xlsx
+++ b/src/test/resources/Datas/Testdatas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7530" tabRatio="948" activeTab="1"/>
+    <workbookView windowWidth="19635" windowHeight="7530" tabRatio="948" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="4" r:id="rId1"/>
@@ -251,7 +251,7 @@
     <t>TargetID</t>
   </si>
   <si>
-    <t>38356</t>
+    <t>15014</t>
   </si>
 </sst>
 </file>
@@ -1432,7 +1432,7 @@
   <sheetPr/>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B11" sqref="B11:D11"/>
     </sheetView>
   </sheetViews>
@@ -2158,8 +2158,8 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
1.Call plan UploadFunction is developed
</commit_message>
<xml_diff>
--- a/src/test/resources/Datas/Testdatas.xlsx
+++ b/src/test/resources/Datas/Testdatas.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="80">
   <si>
     <t>TCID</t>
   </si>
@@ -251,7 +251,16 @@
     <t>TargetID</t>
   </si>
   <si>
-    <t>15014</t>
+    <t>UploadType</t>
+  </si>
+  <si>
+    <t>39419</t>
+  </si>
+  <si>
+    <t>Upload</t>
+  </si>
+  <si>
+    <t>33008</t>
   </si>
 </sst>
 </file>
@@ -964,7 +973,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -972,6 +981,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1347,77 +1359,77 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="44" style="14" customWidth="1"/>
-    <col min="2" max="2" width="16.1238095238095" style="14" customWidth="1"/>
-    <col min="3" max="16384" width="9.14285714285714" style="14"/>
+    <col min="1" max="1" width="44" style="15" customWidth="1"/>
+    <col min="2" max="2" width="16.1238095238095" style="15" customWidth="1"/>
+    <col min="3" max="16384" width="9.14285714285714" style="15"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" spans="1:2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="20.25" spans="1:2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="20.25" spans="1:2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="20.25" spans="1:2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" ht="20.25" spans="1:2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" ht="20.25" spans="1:2">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" ht="20.25" spans="1:2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" ht="20.25" spans="1:2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:2">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1465,186 +1477,186 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" ht="16.5" spans="1:6">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" ht="16.5" spans="1:6">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="12" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" ht="16.5" spans="1:6">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="12" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1687,7 +1699,7 @@
       <c r="B2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1698,7 +1710,7 @@
       <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1709,7 +1721,7 @@
       <c r="B4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1720,7 +1732,7 @@
       <c r="B5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1731,7 +1743,7 @@
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1742,7 +1754,7 @@
       <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1753,7 +1765,7 @@
       <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1764,7 +1776,7 @@
       <c r="B9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1775,7 +1787,7 @@
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1786,7 +1798,7 @@
       <c r="B11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1826,16 +1838,16 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="7" t="b">
+      <c r="C2" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1875,10 +1887,10 @@
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1886,10 +1898,10 @@
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1897,15 +1909,15 @@
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1943,10 +1955,10 @@
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1954,10 +1966,10 @@
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1965,10 +1977,10 @@
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1976,10 +1988,10 @@
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1987,10 +1999,10 @@
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1998,10 +2010,10 @@
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2009,10 +2021,10 @@
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2020,10 +2032,10 @@
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2031,10 +2043,10 @@
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2107,43 +2119,43 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>33456</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="L2" s="5" t="b">
+      <c r="L2" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2156,18 +2168,18 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="2" width="16.8571428571429" customWidth="1"/>
+    <col min="2" max="3" width="16.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2175,17 +2187,37 @@
         <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Call Plan should be optimized for All projects
</commit_message>
<xml_diff>
--- a/src/test/resources/Datas/Testdatas.xlsx
+++ b/src/test/resources/Datas/Testdatas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7530" tabRatio="948" firstSheet="2" activeTab="7"/>
+    <workbookView windowWidth="23040" windowHeight="9144" tabRatio="948" firstSheet="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="87">
   <si>
     <t>TCID</t>
   </si>
@@ -119,6 +119,9 @@
     <t>TC_010</t>
   </si>
   <si>
+    <t>arundel</t>
+  </si>
+  <si>
     <t>Attendancetype</t>
   </si>
   <si>
@@ -254,13 +257,31 @@
     <t>UploadType</t>
   </si>
   <si>
-    <t>39419</t>
+    <t>NetworkMode</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>30566</t>
   </si>
   <si>
     <t>Upload</t>
   </si>
   <si>
-    <t>33008</t>
+    <t>wifi</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>38852</t>
+  </si>
+  <si>
+    <t>Enable</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -273,7 +294,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,13 +331,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Segoe UI"/>
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
-      <sz val="10"/>
+      <sz val="11"/>
       <name val="Segoe UI"/>
       <charset val="134"/>
     </font>
@@ -843,137 +871,137 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -986,9 +1014,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1010,28 +1035,34 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1353,83 +1384,83 @@
   <sheetPr/>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="18" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="44" style="15" customWidth="1"/>
-    <col min="2" max="2" width="16.1238095238095" style="15" customWidth="1"/>
-    <col min="3" max="16384" width="9.14285714285714" style="15"/>
+    <col min="1" max="1" width="44" style="16" customWidth="1"/>
+    <col min="2" max="2" width="16.1203703703704" style="16" customWidth="1"/>
+    <col min="3" max="16384" width="9.13888888888889" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" spans="1:2">
-      <c r="A1" s="16" t="s">
+    <row r="1" ht="20.4" spans="1:2">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="20.25" spans="1:2">
-      <c r="A2" s="17" t="s">
+    <row r="2" ht="20.4" spans="1:2">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" ht="20.25" spans="1:2">
-      <c r="A3" s="17" t="s">
+      <c r="B2" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" ht="20.4" spans="1:2">
+      <c r="A3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="20.25" spans="1:2">
-      <c r="A4" s="17" t="s">
+    <row r="4" ht="20.4" spans="1:2">
+      <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" ht="20.25" spans="1:2">
-      <c r="A5" s="17" t="s">
+    <row r="5" ht="20.4" spans="1:2">
+      <c r="A5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="20.25" spans="1:2">
-      <c r="A6" s="17" t="s">
+    <row r="6" ht="20.4" spans="1:2">
+      <c r="A6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" ht="20.25" spans="1:2">
-      <c r="A7" s="19" t="s">
+    <row r="7" ht="20.4" spans="1:2">
+      <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" ht="20.25" spans="1:2">
-      <c r="A8" s="19" t="s">
+    <row r="8" ht="20.4" spans="1:2">
+      <c r="A8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>3</v>
+      <c r="B8" s="19" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:2">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="16" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1445,218 +1476,220 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D11"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="15.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="15.2857142857143" customWidth="1"/>
-    <col min="5" max="5" width="20.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="9.13888888888889" style="11"/>
+    <col min="2" max="2" width="13" style="11" customWidth="1"/>
+    <col min="3" max="3" width="15.5740740740741" style="11" customWidth="1"/>
+    <col min="4" max="4" width="28.0925925925926" style="11" customWidth="1"/>
+    <col min="5" max="5" width="20.8611111111111" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="9.13888888888889" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="16.8" spans="1:6">
+      <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="12" t="s">
+    <row r="2" ht="16.8" spans="1:6">
+      <c r="A2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="12" t="s">
+    <row r="3" ht="16.8" spans="1:6">
+      <c r="A3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="12" t="s">
+    <row r="4" ht="16.8" spans="1:6">
+      <c r="A4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="12" t="s">
+    <row r="5" ht="16.8" spans="1:6">
+      <c r="A5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="16.5" spans="1:6">
-      <c r="A6" s="12" t="s">
+    <row r="6" ht="16.8" spans="1:6">
+      <c r="A6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="12" t="s">
+    <row r="7" ht="16.8" spans="1:6">
+      <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="12" t="s">
+    <row r="8" ht="16.8" spans="1:6">
+      <c r="A8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" ht="16.5" spans="1:6">
-      <c r="A9" s="12" t="s">
+    <row r="9" ht="16.8" spans="1:6">
+      <c r="A9" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="13" t="s">
+      <c r="E9" s="15"/>
+      <c r="F9" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" ht="16.5" spans="1:6">
-      <c r="A10" s="12" t="s">
+    <row r="10" ht="16.8" spans="1:6">
+      <c r="A10" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="13" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="12" t="s">
+    <row r="11" ht="16.8" spans="1:6">
+      <c r="A11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="B11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1675,18 +1708,18 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="12.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="17.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="12.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="17.8611111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" ht="15" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1697,9 +1730,9 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1708,9 +1741,9 @@
         <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1719,9 +1752,9 @@
         <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1730,9 +1763,9 @@
         <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1741,9 +1774,9 @@
         <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1752,9 +1785,9 @@
         <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1763,9 +1796,9 @@
         <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1774,9 +1807,9 @@
         <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1785,9 +1818,9 @@
         <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1796,9 +1829,9 @@
         <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1814,40 +1847,40 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="3" width="14.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="9.42857142857143" customWidth="1"/>
+    <col min="2" max="3" width="14.8611111111111" customWidth="1"/>
+    <col min="4" max="4" width="9.42592592592593" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" ht="15" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="8" t="b">
+      <c r="B2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1863,21 +1896,21 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="17.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="17.1388888888889" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" ht="15" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1887,10 +1920,10 @@
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1898,10 +1931,10 @@
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1909,15 +1942,15 @@
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="10"/>
+      <c r="A5" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1934,18 +1967,18 @@
       <selection activeCell="A1" sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="40.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="11.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="40.1388888888889" customWidth="1"/>
+    <col min="3" max="3" width="11.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" ht="15" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1955,10 +1988,10 @@
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1966,10 +1999,10 @@
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1977,10 +2010,10 @@
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1988,10 +2021,10 @@
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1999,10 +2032,10 @@
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2010,10 +2043,10 @@
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2021,10 +2054,10 @@
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2032,10 +2065,10 @@
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2043,10 +2076,10 @@
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2065,97 +2098,97 @@
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
-    <col min="2" max="2" width="10.4190476190476" customWidth="1"/>
+    <col min="2" max="2" width="10.4166666666667" customWidth="1"/>
     <col min="3" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="55.8" customWidth="1"/>
-    <col min="9" max="9" width="19.5714285714286" customWidth="1"/>
-    <col min="10" max="10" width="21.8571428571429" customWidth="1"/>
-    <col min="11" max="11" width="27.5714285714286" customWidth="1"/>
+    <col min="8" max="8" width="55.7962962962963" customWidth="1"/>
+    <col min="9" max="9" width="19.5740740740741" customWidth="1"/>
+    <col min="10" max="10" width="21.8611111111111" customWidth="1"/>
+    <col min="11" max="11" width="27.5740740740741" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="11.9333333333333" customWidth="1"/>
+    <col min="13" max="13" width="11.9351851851852" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" ht="15" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="6">
+      <c r="C2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="5">
         <v>33456</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="L2" s="6" t="b">
+      <c r="I2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2168,56 +2201,74 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
-    <col min="2" max="3" width="16.8571428571429" customWidth="1"/>
+    <col min="2" max="5" width="16.8611111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" ht="15" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>80</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TestLogs Developed in Call plan Module
</commit_message>
<xml_diff>
--- a/src/test/resources/Datas/Testdatas.xlsx
+++ b/src/test/resources/Datas/Testdatas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9144" tabRatio="948" firstSheet="2" activeTab="1"/>
+    <workbookView windowWidth="19635" windowHeight="7530" tabRatio="948" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="87">
   <si>
     <t>TCID</t>
   </si>
@@ -116,9 +116,6 @@
     <t>TC_010</t>
   </si>
   <si>
-    <t>USARA</t>
-  </si>
-  <si>
     <t>jj</t>
   </si>
   <si>
@@ -272,7 +269,7 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>36831</t>
+    <t>37248</t>
   </si>
   <si>
     <t>Upload</t>
@@ -1445,17 +1442,17 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A32"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="18" outlineLevelRow="7" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelRow="7" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="54.9166666666667" style="23" customWidth="1"/>
-    <col min="2" max="2" width="30.1574074074074" style="23" customWidth="1"/>
-    <col min="3" max="16384" width="9.13888888888889" style="23"/>
+    <col min="1" max="1" width="54.9142857142857" style="23" customWidth="1"/>
+    <col min="2" max="2" width="30.1619047619048" style="23" customWidth="1"/>
+    <col min="3" max="16384" width="9.14285714285714" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" spans="1:2">
+    <row r="1" ht="26.25" spans="1:2">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1463,7 +1460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="27" spans="1:2">
+    <row r="2" ht="26.25" spans="1:2">
       <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
@@ -1471,7 +1468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="27" spans="1:2">
+    <row r="3" ht="26.25" spans="1:2">
       <c r="A3" s="25" t="s">
         <v>4</v>
       </c>
@@ -1479,7 +1476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" ht="27" spans="1:2">
+    <row r="4" ht="26.25" spans="1:2">
       <c r="A4" s="25" t="s">
         <v>5</v>
       </c>
@@ -1487,7 +1484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="27" spans="1:2">
+    <row r="5" ht="26.25" spans="1:2">
       <c r="A5" s="25" t="s">
         <v>7</v>
       </c>
@@ -1495,7 +1492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" ht="27" spans="1:2">
+    <row r="6" ht="26.25" spans="1:2">
       <c r="A6" s="25" t="s">
         <v>8</v>
       </c>
@@ -1503,7 +1500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" ht="27" spans="1:2">
+    <row r="7" ht="26.25" spans="1:2">
       <c r="A7" s="27" t="s">
         <v>9</v>
       </c>
@@ -1511,7 +1508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" ht="27" spans="1:2">
+    <row r="8" ht="26.25" spans="1:2">
       <c r="A8" s="27" t="s">
         <v>10</v>
       </c>
@@ -1530,22 +1527,22 @@
   <sheetPr/>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.5092592592593" style="19" customWidth="1"/>
+    <col min="1" max="1" width="14.5047619047619" style="19" customWidth="1"/>
     <col min="2" max="2" width="13" style="19" customWidth="1"/>
-    <col min="3" max="3" width="15.5740740740741" style="19" customWidth="1"/>
-    <col min="4" max="4" width="28.0925925925926" style="19" customWidth="1"/>
-    <col min="5" max="5" width="20.8611111111111" style="19" customWidth="1"/>
-    <col min="6" max="6" width="17.7777777777778" style="19" customWidth="1"/>
-    <col min="7" max="16384" width="9.13888888888889" style="19"/>
+    <col min="3" max="3" width="15.5714285714286" style="19" customWidth="1"/>
+    <col min="4" max="4" width="28.0952380952381" style="19" customWidth="1"/>
+    <col min="5" max="5" width="20.8571428571429" style="19" customWidth="1"/>
+    <col min="6" max="6" width="17.7809523809524" style="19" customWidth="1"/>
+    <col min="7" max="16384" width="9.14285714285714" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" spans="1:6">
+    <row r="1" ht="18.75" spans="1:6">
       <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
@@ -1565,7 +1562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="18" spans="1:6">
+    <row r="2" ht="18.75" spans="1:6">
       <c r="A2" s="20" t="s">
         <v>16</v>
       </c>
@@ -1585,7 +1582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="18" spans="1:6">
+    <row r="3" ht="18.75" spans="1:6">
       <c r="A3" s="20" t="s">
         <v>21</v>
       </c>
@@ -1605,7 +1602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" ht="18" spans="1:6">
+    <row r="4" ht="18.75" spans="1:6">
       <c r="A4" s="20" t="s">
         <v>22</v>
       </c>
@@ -1625,7 +1622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="18" spans="1:6">
+    <row r="5" ht="18.75" spans="1:6">
       <c r="A5" s="20" t="s">
         <v>24</v>
       </c>
@@ -1645,7 +1642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" ht="18" spans="1:6">
+    <row r="6" ht="18.75" spans="1:6">
       <c r="A6" s="20" t="s">
         <v>25</v>
       </c>
@@ -1663,7 +1660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" ht="18" spans="1:6">
+    <row r="7" ht="18.75" spans="1:6">
       <c r="A7" s="20" t="s">
         <v>26</v>
       </c>
@@ -1681,7 +1678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" ht="18" spans="1:6">
+    <row r="8" ht="18.75" spans="1:6">
       <c r="A8" s="20" t="s">
         <v>27</v>
       </c>
@@ -1699,7 +1696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" ht="18" spans="1:6">
+    <row r="9" ht="18.75" spans="1:6">
       <c r="A9" s="20" t="s">
         <v>28</v>
       </c>
@@ -1717,7 +1714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" ht="18" spans="1:6">
+    <row r="10" ht="18.75" spans="1:6">
       <c r="A10" s="20" t="s">
         <v>29</v>
       </c>
@@ -1729,18 +1726,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" ht="18" spans="1:6">
+    <row r="11" ht="18.75" spans="1:6">
       <c r="A11" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>20</v>
@@ -1764,129 +1761,129 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="12.712962962963" customWidth="1"/>
-    <col min="2" max="2" width="22.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="13.8888888888889" customWidth="1"/>
+    <col min="1" max="1" width="12.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="22.7809523809524" customWidth="1"/>
+    <col min="3" max="3" width="13.8857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" spans="1:3">
+    <row r="1" ht="18.75" spans="1:3">
       <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="18" spans="1:3">
+    <row r="2" ht="18.75" spans="1:3">
       <c r="A2" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="18" spans="1:3">
+    <row r="3" ht="18.75" spans="1:3">
       <c r="A3" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" ht="18" spans="1:3">
+    <row r="4" ht="18.75" spans="1:3">
       <c r="A4" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" ht="18" spans="1:3">
+    <row r="5" ht="18.75" spans="1:3">
       <c r="A5" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" ht="18" spans="1:3">
+    <row r="6" ht="18.75" spans="1:3">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" ht="18" spans="1:3">
+    <row r="7" ht="18.75" spans="1:3">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" ht="18" spans="1:3">
+    <row r="8" ht="18.75" spans="1:3">
       <c r="A8" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" ht="18" spans="1:3">
+    <row r="9" ht="18.75" spans="1:3">
       <c r="A9" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" ht="18" spans="1:3">
+    <row r="10" ht="18.75" spans="1:3">
       <c r="A10" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" ht="18" spans="1:3">
+    <row r="11" ht="18.75" spans="1:3">
       <c r="A11" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>3</v>
@@ -1907,34 +1904,34 @@
       <selection activeCell="E10" sqref="A1:D2 E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="9.44444444444444" customWidth="1"/>
-    <col min="2" max="2" width="22.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="9.44761904761905" customWidth="1"/>
+    <col min="2" max="2" width="22.1142857142857" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="13.8888888888889" customWidth="1"/>
+    <col min="4" max="4" width="13.8857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" spans="1:4">
+    <row r="1" ht="18.75" spans="1:4">
       <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="18" spans="1:4">
+    <row r="2" ht="18.75" spans="1:4">
       <c r="A2" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="11" t="b">
         <v>1</v>
@@ -1958,51 +1955,51 @@
       <selection activeCell="G5" sqref="A1:C4 G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="17.1388888888889" customWidth="1"/>
+    <col min="2" max="2" width="17.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" spans="1:3">
+    <row r="1" ht="18.75" spans="1:3">
       <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="18" spans="1:3">
+    <row r="2" ht="18.75" spans="1:3">
       <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="18" spans="1:3">
+    <row r="3" ht="18.75" spans="1:3">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" ht="18" spans="1:3">
+    <row r="4" ht="18.75" spans="1:3">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>3</v>
@@ -2026,117 +2023,117 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="40.1388888888889" customWidth="1"/>
-    <col min="3" max="3" width="11.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="40.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="11.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.4" spans="1:3">
+    <row r="1" ht="20.25" spans="1:3">
       <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="18" spans="1:3">
+    <row r="2" ht="18.75" spans="1:3">
       <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="18" spans="1:3">
+    <row r="3" ht="18.75" spans="1:3">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" ht="18" spans="1:3">
+    <row r="4" ht="18.75" spans="1:3">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" ht="18" spans="1:3">
+    <row r="5" ht="18.75" spans="1:3">
       <c r="A5" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" ht="18" spans="1:3">
+    <row r="6" ht="18.75" spans="1:3">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" ht="18" spans="1:3">
+    <row r="7" ht="18.75" spans="1:3">
       <c r="A7" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" ht="18" spans="1:3">
+    <row r="8" ht="18.75" spans="1:3">
       <c r="A8" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" ht="18" spans="1:3">
+    <row r="9" ht="18.75" spans="1:3">
       <c r="A9" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" ht="18" spans="1:3">
+    <row r="10" ht="18.75" spans="1:3">
       <c r="A10" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>3</v>
@@ -2157,92 +2154,92 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="2" max="2" width="10.4166666666667" customWidth="1"/>
+    <col min="2" max="2" width="10.4190476190476" customWidth="1"/>
     <col min="3" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="55.7962962962963" customWidth="1"/>
-    <col min="9" max="9" width="19.5740740740741" customWidth="1"/>
-    <col min="10" max="10" width="21.8611111111111" customWidth="1"/>
-    <col min="11" max="11" width="27.5740740740741" customWidth="1"/>
+    <col min="8" max="8" width="55.8" customWidth="1"/>
+    <col min="9" max="9" width="19.5714285714286" customWidth="1"/>
+    <col min="10" max="10" width="21.8571428571429" customWidth="1"/>
+    <col min="11" max="11" width="27.5714285714286" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="11.9351851851852" customWidth="1"/>
+    <col min="13" max="13" width="11.9333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36" spans="1:13">
+    <row r="1" ht="37.5" spans="1:13">
       <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="18" spans="1:13">
+    <row r="2" ht="18.75" spans="1:13">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="D2" s="7">
         <v>33456</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>75</v>
-      </c>
       <c r="J2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L2" s="7" t="b">
         <v>1</v>
@@ -2262,47 +2259,47 @@
   <sheetPr/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="9.13888888888889" style="1"/>
-    <col min="2" max="3" width="16.8611111111111" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.14285714285714" style="1"/>
+    <col min="2" max="3" width="16.8571428571429" style="1" customWidth="1"/>
     <col min="4" max="4" width="27.6666666666667" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.4444444444444" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.1111111111111" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.447619047619" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1142857142857" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.6666666666667" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.8611111111111" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.8571428571429" style="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.13888888888889" style="1"/>
+    <col min="10" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.2" spans="1:9">
+    <row r="1" ht="17.25" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>1</v>
@@ -2313,25 +2310,25 @@
         <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Query Should be Modified
</commit_message>
<xml_diff>
--- a/src/test/resources/Datas/Testdatas.xlsx
+++ b/src/test/resources/Datas/Testdatas.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="101">
   <si>
     <t>TCID</t>
   </si>
@@ -116,6 +116,9 @@
     <t>TC_010</t>
   </si>
   <si>
+    <t>Gunache</t>
+  </si>
+  <si>
     <t>jj</t>
   </si>
   <si>
@@ -269,7 +272,7 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>37248</t>
+    <t>36679</t>
   </si>
   <si>
     <t>Upload</t>
@@ -281,7 +284,46 @@
     <t>Mandatory</t>
   </si>
   <si>
+    <t>wifi</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>36676</t>
+  </si>
+  <si>
     <t>Enable</t>
+  </si>
+  <si>
+    <t>36680</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>36674</t>
+  </si>
+  <si>
+    <t>36114</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Permanently Store Closed</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>25668</t>
+  </si>
+  <si>
+    <t>38556</t>
   </si>
 </sst>
 </file>
@@ -1441,8 +1483,8 @@
   <sheetPr/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelRow="7" outlineLevelCol="1"/>
@@ -1528,7 +1570,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1731,13 +1773,13 @@
         <v>30</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>20</v>
@@ -1773,7 +1815,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>1</v>
@@ -1784,7 +1826,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3</v>
@@ -1795,7 +1837,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>3</v>
@@ -1806,7 +1848,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>3</v>
@@ -1817,7 +1859,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>3</v>
@@ -1828,7 +1870,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>3</v>
@@ -1839,7 +1881,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>3</v>
@@ -1850,7 +1892,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>3</v>
@@ -1861,7 +1903,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>6</v>
@@ -1872,7 +1914,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>3</v>
@@ -1883,7 +1925,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>3</v>
@@ -1917,10 +1959,10 @@
         <v>11</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>1</v>
@@ -1931,7 +1973,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="11" t="b">
         <v>1</v>
@@ -1966,7 +2008,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>1</v>
@@ -1977,7 +2019,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>3</v>
@@ -1988,7 +2030,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>3</v>
@@ -1999,7 +2041,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>3</v>
@@ -2034,7 +2076,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>1</v>
@@ -2045,7 +2087,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>3</v>
@@ -2056,7 +2098,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>3</v>
@@ -2067,7 +2109,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>3</v>
@@ -2078,7 +2120,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>3</v>
@@ -2089,7 +2131,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>3</v>
@@ -2100,7 +2142,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>3</v>
@@ -2111,7 +2153,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>3</v>
@@ -2122,7 +2164,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>3</v>
@@ -2133,7 +2175,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>3</v>
@@ -2171,37 +2213,37 @@
         <v>11</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>1</v>
@@ -2212,34 +2254,34 @@
         <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D2" s="7">
         <v>33456</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L2" s="7" t="b">
         <v>1</v>
@@ -2257,13 +2299,13 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="9.14285714285714" style="1"/>
     <col min="2" max="3" width="16.8571428571429" style="1" customWidth="1"/>
@@ -2281,25 +2323,25 @@
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>1</v>
@@ -2310,27 +2352,201 @@
         <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:9">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:9">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="E4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:9">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" spans="1:9">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" spans="1:9">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="D7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" spans="1:9">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Attendance Test should be Validate
</commit_message>
<xml_diff>
--- a/src/test/resources/Datas/Testdatas.xlsx
+++ b/src/test/resources/Datas/Testdatas.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation Workspace\FrameXMobile_V1.0\src\test\resources\Datas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BD8CEC-B09F-49F2-8B0A-94F12C95E59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7530" tabRatio="948" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="948" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="4" r:id="rId1"/>
@@ -116,9 +122,6 @@
     <t>TC_010</t>
   </si>
   <si>
-    <t>Gunache</t>
-  </si>
-  <si>
     <t>jj</t>
   </si>
   <si>
@@ -272,9 +275,6 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>36679</t>
-  </si>
-  <si>
     <t>Upload</t>
   </si>
   <si>
@@ -308,9 +308,6 @@
     <t>36674</t>
   </si>
   <si>
-    <t>36114</t>
-  </si>
-  <si>
     <t>Close</t>
   </si>
   <si>
@@ -324,19 +321,22 @@
   </si>
   <si>
     <t>38556</t>
+  </si>
+  <si>
+    <t>33114</t>
+  </si>
+  <si>
+    <t>31083</t>
+  </si>
+  <si>
+    <t>600</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="35">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,7 +347,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1" tint="0.05"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Segoe UI"/>
       <charset val="134"/>
     </font>
@@ -445,152 +445,8 @@
       <name val="Segoe UI Semibold"/>
       <charset val="134"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -605,7 +461,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.25"/>
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -627,188 +483,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -831,255 +507,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1137,9 +571,6 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1163,61 +594,17 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1475,116 +862,113 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="51" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="18.75" outlineLevelRow="7" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="54.9142857142857" style="23" customWidth="1"/>
-    <col min="2" max="2" width="30.1619047619048" style="23" customWidth="1"/>
-    <col min="3" max="16384" width="9.14285714285714" style="23"/>
+    <col min="1" max="1" width="54.85546875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="22" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26.25" spans="1:2">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:2" ht="26.25">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="26.25" spans="1:2">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:2" ht="26.25">
+      <c r="A2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" ht="26.25" spans="1:2">
-      <c r="A3" s="25" t="s">
+      <c r="B2" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="26.25">
+      <c r="A3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" ht="26.25" spans="1:2">
-      <c r="A4" s="25" t="s">
+      <c r="B3" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="26.25">
+      <c r="A4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" ht="26.25" spans="1:2">
-      <c r="A5" s="25" t="s">
+      <c r="B4" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="26.25">
+      <c r="A5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" ht="26.25" spans="1:2">
-      <c r="A6" s="25" t="s">
+      <c r="B5" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="26.25">
+      <c r="A6" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" ht="26.25" spans="1:2">
-      <c r="A7" s="27" t="s">
+      <c r="B6" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="26.25">
+      <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" ht="26.25" spans="1:2">
-      <c r="A8" s="27" t="s">
+      <c r="B7" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="26.25">
+      <c r="A8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5047619047619" style="19" customWidth="1"/>
-    <col min="2" max="2" width="13" style="19" customWidth="1"/>
-    <col min="3" max="3" width="15.5714285714286" style="19" customWidth="1"/>
-    <col min="4" max="4" width="28.0952380952381" style="19" customWidth="1"/>
-    <col min="5" max="5" width="20.8571428571429" style="19" customWidth="1"/>
-    <col min="6" max="6" width="17.7809523809524" style="19" customWidth="1"/>
-    <col min="7" max="16384" width="9.14285714285714" style="19"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" spans="1:6">
+    <row r="1" spans="1:6" ht="18.75">
       <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
@@ -1604,328 +988,326 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="18.75" spans="1:6">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:6" ht="18.75">
+      <c r="A2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" ht="18.75" spans="1:6">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:6" ht="18.75">
+      <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" ht="18.75" spans="1:6">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:6" ht="18.75">
+      <c r="A4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" ht="18.75" spans="1:6">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:6" ht="18.75">
+      <c r="A5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" ht="18.75" spans="1:6">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:6" ht="18.75">
+      <c r="A6" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="20" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" ht="18.75" spans="1:6">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:6" ht="18.75">
+      <c r="A7" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" ht="18.75" spans="1:6">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:6" ht="18.75">
+      <c r="A8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20" t="s">
+      <c r="D8" s="19"/>
+      <c r="E8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" ht="18.75" spans="1:6">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:6" ht="18.75">
+      <c r="A9" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="21" t="s">
+      <c r="E9" s="21"/>
+      <c r="F9" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" ht="18.75" spans="1:6">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:6" ht="18.75">
+      <c r="A10" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="21" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" ht="18.75" spans="1:6">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:6" ht="18.75">
+      <c r="A11" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="20" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="22.7809523809524" customWidth="1"/>
-    <col min="3" max="3" width="13.8857142857143" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" spans="1:3">
+    <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="18.75" spans="1:3">
+    <row r="2" spans="1:3" ht="18.75">
       <c r="A2" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="18.75" spans="1:3">
+    <row r="3" spans="1:3" ht="18.75">
       <c r="A3" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" ht="18.75" spans="1:3">
+    <row r="4" spans="1:3" ht="18.75">
       <c r="A4" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" ht="18.75" spans="1:3">
+    <row r="5" spans="1:3" ht="18.75">
       <c r="A5" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" ht="18.75" spans="1:3">
+    <row r="6" spans="1:3" ht="18.75">
       <c r="A6" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" ht="18.75" spans="1:3">
+    <row r="7" spans="1:3" ht="18.75">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" ht="18.75" spans="1:3">
+    <row r="8" spans="1:3" ht="18.75">
       <c r="A8" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" ht="18.75" spans="1:3">
+    <row r="9" spans="1:3" ht="18.75">
       <c r="A9" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" ht="18.75" spans="1:3">
+    <row r="10" spans="1:3" ht="18.75">
       <c r="A10" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" ht="18.75" spans="1:3">
+    <row r="11" spans="1:3" ht="18.75">
       <c r="A11" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>3</v>
@@ -1933,47 +1315,45 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="A1:D2 E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.44761904761905" customWidth="1"/>
-    <col min="2" max="2" width="22.1142857142857" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="13.8857142857143" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" spans="1:4">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="18.75" spans="1:4">
+    <row r="2" spans="1:4" ht="18.75">
       <c r="A2" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="11" t="b">
         <v>1</v>
@@ -1984,198 +1364,194 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="A1:C4 G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" spans="1:3">
+    <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="18.75" spans="1:3">
+    <row r="2" spans="1:3" ht="18.75">
       <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="18.75" spans="1:3">
+    <row r="3" spans="1:3" ht="18.75">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" ht="18.75" spans="1:3">
+    <row r="4" spans="1:3" ht="18.75">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:3">
       <c r="A5" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="40.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="11.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" spans="1:3">
+    <row r="1" spans="1:3" ht="20.25">
       <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="18.75" spans="1:3">
+    <row r="2" spans="1:3" ht="18.75">
       <c r="A2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="18.75" spans="1:3">
+    <row r="3" spans="1:3" ht="18.75">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" ht="18.75" spans="1:3">
+    <row r="4" spans="1:3" ht="18.75">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" ht="18.75" spans="1:3">
+    <row r="5" spans="1:3" ht="18.75">
       <c r="A5" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" ht="18.75" spans="1:3">
+    <row r="6" spans="1:3" ht="18.75">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" ht="18.75" spans="1:3">
+    <row r="7" spans="1:3" ht="18.75">
       <c r="A7" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" ht="18.75" spans="1:3">
+    <row r="8" spans="1:3" ht="18.75">
       <c r="A8" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" ht="18.75" spans="1:3">
+    <row r="9" spans="1:3" ht="18.75">
       <c r="A9" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" ht="18.75" spans="1:3">
+    <row r="10" spans="1:3" ht="18.75">
       <c r="A10" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>3</v>
@@ -2183,105 +1559,105 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="64" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.4190476190476" customWidth="1"/>
-    <col min="3" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="55.8" customWidth="1"/>
-    <col min="9" max="9" width="19.5714285714286" customWidth="1"/>
-    <col min="10" max="10" width="21.8571428571429" customWidth="1"/>
-    <col min="11" max="11" width="27.5714285714286" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="55.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="11.9333333333333" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="37.5" spans="1:13">
+    <row r="1" spans="1:13" ht="37.5">
       <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="18.75" spans="1:13">
+    <row r="2" spans="1:13" ht="18.75">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="D2" s="7">
         <v>33456</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>75</v>
-      </c>
       <c r="J2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L2" s="7" t="b">
         <v>1</v>
@@ -2292,91 +1668,89 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" style="1"/>
-    <col min="2" max="3" width="16.8571428571429" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.6666666666667" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.447619047619" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.1142857142857" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6666666666667" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.8571428571429" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="3" width="16.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.14285714285714" style="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" spans="1:9">
+    <row r="1" spans="1:9" ht="17.25">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="19" customHeight="1" spans="1:9">
+    <row r="2" spans="1:9" ht="18.95" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="1:9">
+    <row r="3" spans="1:9" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -2384,174 +1758,173 @@
         <v>89</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="1:9">
+    <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="I4" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" spans="1:9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" spans="1:9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" spans="1:9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="G7" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" spans="1:9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="G8" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>